<commit_message>
Added option to create info plots of any time window, add up to two markers
</commit_message>
<xml_diff>
--- a/data/Cougars_ODBA_KIlls_Setup.xlsx
+++ b/data/Cougars_ODBA_KIlls_Setup.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSU\AI Capstone\ai-capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CEA40F-0739-41A1-9A0E-7AE6F6D5FB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83181875-5609-4A11-B3B7-C3547646D856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="624" windowWidth="22680" windowHeight="11616" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="624" windowWidth="22680" windowHeight="11616" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="M201" sheetId="1" r:id="rId1"/>
-    <sheet name="F202" sheetId="2" r:id="rId2"/>
-    <sheet name="AllCats" sheetId="3" r:id="rId3"/>
-    <sheet name="F202Kills2" sheetId="4" r:id="rId4"/>
-    <sheet name="F202Kills" sheetId="5" r:id="rId5"/>
-    <sheet name="F209" sheetId="6" r:id="rId6"/>
-    <sheet name="F209Kills" sheetId="7" r:id="rId7"/>
-    <sheet name="F207" sheetId="8" r:id="rId8"/>
-    <sheet name="F207Kills" sheetId="9" r:id="rId9"/>
+    <sheet name="InfoPlots" sheetId="10" r:id="rId1"/>
+    <sheet name="M201" sheetId="1" r:id="rId2"/>
+    <sheet name="F202" sheetId="2" r:id="rId3"/>
+    <sheet name="AllCats" sheetId="3" r:id="rId4"/>
+    <sheet name="F202Kills2" sheetId="4" r:id="rId5"/>
+    <sheet name="F202Kills" sheetId="5" r:id="rId6"/>
+    <sheet name="F209" sheetId="6" r:id="rId7"/>
+    <sheet name="F209Kills" sheetId="7" r:id="rId8"/>
+    <sheet name="F207" sheetId="8" r:id="rId9"/>
+    <sheet name="F207Kills" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13863" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13882" uniqueCount="1038">
   <si>
     <t>AnimalID</t>
   </si>
@@ -3539,6 +3540,42 @@
   <si>
     <t>StartKill</t>
   </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>MarkerTime2</t>
+  </si>
+  <si>
+    <t>MarkerLabel1</t>
+  </si>
+  <si>
+    <t>MarkerLabel2</t>
+  </si>
+  <si>
+    <t>PlotLabel</t>
+  </si>
+  <si>
+    <t>Long Kill Window</t>
+  </si>
+  <si>
+    <t>MarkerTime1</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>KillEndPhase2</t>
+  </si>
+  <si>
+    <t>2nd Marker (demo)</t>
+  </si>
+  <si>
+    <t>UpdatedStartStalk</t>
+  </si>
+  <si>
+    <t>Long Stalk Window</t>
+  </si>
 </sst>
 </file>
 
@@ -3548,7 +3585,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -3612,6 +3649,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3681,7 +3731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3798,6 +3848,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4179,6 +4235,2101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE45E2E-6649-4C29-87B5-2DB9979F8950}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>1033</v>
+      </c>
+      <c r="G1" s="55" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H1" s="55" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I1" s="55" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J1" s="55" t="s">
+        <v>1029</v>
+      </c>
+      <c r="K1" s="55" t="s">
+        <v>1030</v>
+      </c>
+      <c r="L1" s="55" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="8">
+        <v>202</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10">
+        <v>976</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43183</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="F2" s="56">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="G2" s="53">
+        <v>0.39303240740740741</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I2" s="57">
+        <v>0.39354166666666668</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>976</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43183</v>
+      </c>
+      <c r="E3" s="56">
+        <v>0.375</v>
+      </c>
+      <c r="F3" s="56">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="G3" s="57">
+        <v>0.37677083333333333</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="F6" s="54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:U31"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="36" customFormat="1">
+      <c r="A2" s="31">
+        <v>10</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>909</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>496</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="33">
+        <v>42804</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="34">
+        <v>42835</v>
+      </c>
+      <c r="L2" s="35">
+        <v>2017</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>929</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>930</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>931</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="36" t="str">
+        <f t="shared" ref="U2:U31" si="0">CONCATENATE("12N ",O2,"mE ",P2,"mN")</f>
+        <v>12N 529588mE 4969531mN</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="27" customFormat="1">
+      <c r="A3" s="22">
+        <v>15</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="24">
+        <v>42807</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K3" s="25">
+        <v>42816</v>
+      </c>
+      <c r="L3" s="26">
+        <v>2017</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>932</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>933</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23" t="s">
+        <v>434</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="T3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 527518mE 4977401mN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="27" customFormat="1">
+      <c r="A4" s="22">
+        <v>28</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>911</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="24">
+        <v>42819</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="25">
+        <v>42831</v>
+      </c>
+      <c r="L4" s="26">
+        <v>2017</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>935</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>936</v>
+      </c>
+      <c r="P4" s="23" t="s">
+        <v>937</v>
+      </c>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23" t="s">
+        <v>434</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>938</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 540556mE 4978867mN</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="27" customFormat="1">
+      <c r="A5" s="22">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>912</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="24">
+        <v>42866</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K5" s="25">
+        <v>42894</v>
+      </c>
+      <c r="L5" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M5" s="22">
+        <v>3</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>940</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>941</v>
+      </c>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S5" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="T5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 539920mE 4963374mN</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="27" customFormat="1">
+      <c r="A6" s="22">
+        <v>6</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>913</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="24">
+        <v>42878</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="25">
+        <v>42886</v>
+      </c>
+      <c r="L6" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M6" s="22">
+        <v>4</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>942</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>943</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>944</v>
+      </c>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 543511mE 4963289mN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="27" customFormat="1">
+      <c r="A7" s="22">
+        <v>8</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>945</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="24">
+        <v>42879</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K7" s="25">
+        <v>42886</v>
+      </c>
+      <c r="L7" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M7" s="22">
+        <v>17</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>946</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>947</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>948</v>
+      </c>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S7" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="T7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 543062mE 4962326mN</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="27" customFormat="1">
+      <c r="A8" s="22">
+        <v>14</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>914</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="24">
+        <v>42888</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K8" s="25">
+        <v>42942</v>
+      </c>
+      <c r="L8" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M8" s="22">
+        <v>1</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>949</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>950</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>951</v>
+      </c>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="S8" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 530296mE 4961770mN</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="27" customFormat="1">
+      <c r="A9" s="22">
+        <v>15</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>915</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="24">
+        <v>42893</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K9" s="25">
+        <v>42906</v>
+      </c>
+      <c r="L9" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M9" s="22">
+        <v>6</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>952</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>954</v>
+      </c>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U9" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 528094mE 4955737mN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="27" customFormat="1">
+      <c r="A10" s="22">
+        <v>15</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>916</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="24">
+        <v>42893</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K10" s="25">
+        <v>42906</v>
+      </c>
+      <c r="L10" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>952</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>954</v>
+      </c>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S10" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U10" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 528094mE 4955737mN</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="27" customFormat="1">
+      <c r="A11" s="22">
+        <v>18</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>917</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="24">
+        <v>42897</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K11" s="25">
+        <v>42906</v>
+      </c>
+      <c r="L11" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M11" s="22">
+        <v>0</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>955</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>956</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>957</v>
+      </c>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U11" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 526859mE 4955914mN</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="36" customFormat="1">
+      <c r="A12" s="31">
+        <v>20</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>919</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>496</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="33">
+        <v>42905</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="K12" s="34">
+        <v>42922</v>
+      </c>
+      <c r="L12" s="35">
+        <v>2017</v>
+      </c>
+      <c r="M12" s="31">
+        <v>8</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>958</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>959</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="S12" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="T12" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="U12" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 527423mE 4962748mN</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="27" customFormat="1">
+      <c r="A13" s="22">
+        <v>22</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>918</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="24">
+        <v>42904</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="25">
+        <v>42943</v>
+      </c>
+      <c r="L13" s="26">
+        <v>2017</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>949</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>961</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>962</v>
+      </c>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U13" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 529990mE 4965163mN</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="27" customFormat="1">
+      <c r="A14" s="22">
+        <v>23</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>920</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="24">
+        <v>42906</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" s="25">
+        <v>42922</v>
+      </c>
+      <c r="L14" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M14" s="22">
+        <v>5</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>963</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>964</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S14" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="T14" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U14" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 526710mE 4963093mN</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="27" customFormat="1">
+      <c r="A15" s="22">
+        <v>23</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="24">
+        <v>42906</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" s="25">
+        <v>42922</v>
+      </c>
+      <c r="L15" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>963</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>966</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>967</v>
+      </c>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U15" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 526790mE 4963181mN</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="27" customFormat="1">
+      <c r="A16" s="22">
+        <v>30</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="24">
+        <v>42913</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="25">
+        <v>42929</v>
+      </c>
+      <c r="L16" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M16" s="22">
+        <v>0</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>968</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>969</v>
+      </c>
+      <c r="P16" s="23" t="s">
+        <v>970</v>
+      </c>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="S16" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U16" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 527049mE 4957506mN</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="27" customFormat="1">
+      <c r="A17" s="22">
+        <v>33</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>923</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="24">
+        <v>42918</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K17" s="25">
+        <v>42922</v>
+      </c>
+      <c r="L17" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>972</v>
+      </c>
+      <c r="P17" s="23" t="s">
+        <v>973</v>
+      </c>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="S17" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 524166mE 4964425mN</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="27" customFormat="1">
+      <c r="A18" s="22">
+        <v>38</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>924</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="24">
+        <v>42922</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" s="25">
+        <v>42929</v>
+      </c>
+      <c r="L18" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>974</v>
+      </c>
+      <c r="O18" s="23" t="s">
+        <v>975</v>
+      </c>
+      <c r="P18" s="23" t="s">
+        <v>976</v>
+      </c>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="S18" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U18" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 526257mE 4955599mN</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="27" customFormat="1">
+      <c r="A19" s="22">
+        <v>41</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>925</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="24">
+        <v>42928</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K19" s="25">
+        <v>42941</v>
+      </c>
+      <c r="L19" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M19" s="22">
+        <v>4</v>
+      </c>
+      <c r="N19" s="23" t="s">
+        <v>977</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>978</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="S19" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="T19" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U19" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 533197mE 4958093mN</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="27" customFormat="1">
+      <c r="A20" s="22">
+        <v>41</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>926</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="24">
+        <v>42928</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="K20" s="25">
+        <v>42941</v>
+      </c>
+      <c r="L20" s="26">
+        <v>2017</v>
+      </c>
+      <c r="M20" s="22">
+        <v>0</v>
+      </c>
+      <c r="N20" s="23" t="s">
+        <v>980</v>
+      </c>
+      <c r="O20" s="23" t="s">
+        <v>981</v>
+      </c>
+      <c r="P20" s="23" t="s">
+        <v>982</v>
+      </c>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="S20" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="T20" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U20" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 533309mE 4958115mN</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="10">
+        <v>15</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>983</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="28">
+        <v>43071</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="K21" s="29">
+        <v>43079</v>
+      </c>
+      <c r="L21" s="30">
+        <v>2017</v>
+      </c>
+      <c r="M21" s="10">
+        <v>15</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>929</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>984</v>
+      </c>
+      <c r="P21" s="14" t="s">
+        <v>985</v>
+      </c>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 529467mE 4970128mN</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>986</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="28">
+        <v>43133</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="29">
+        <v>43160</v>
+      </c>
+      <c r="L22" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M22" s="10">
+        <v>57</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>987</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>988</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>989</v>
+      </c>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 533055mE 4970931mN</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="10">
+        <v>10</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>990</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="28">
+        <v>43156</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K23" s="29">
+        <v>43168</v>
+      </c>
+      <c r="L23" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M23" s="10">
+        <v>9</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>991</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>992</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>993</v>
+      </c>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14" t="s">
+        <v>994</v>
+      </c>
+      <c r="S23" s="14" t="s">
+        <v>995</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 546430mE 4969479mN</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="10">
+        <v>18</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>927</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="28">
+        <v>43173</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K24" s="29">
+        <v>43182</v>
+      </c>
+      <c r="L24" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M24" s="10">
+        <v>610</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>996</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>997</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="Q24" s="14"/>
+      <c r="T24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 545270mE 4972924mN</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="10">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>999</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="28">
+        <v>43177</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K25" s="29">
+        <v>43182</v>
+      </c>
+      <c r="L25" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M25" s="10">
+        <v>0</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>1001</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Q25" s="14"/>
+      <c r="T25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 542618mE 4975375mN</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="10">
+        <v>22</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="28">
+        <v>43182</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="29">
+        <v>43187</v>
+      </c>
+      <c r="L26" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M26" s="10">
+        <v>510</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="O26" s="14" t="s">
+        <v>1005</v>
+      </c>
+      <c r="P26" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 542398mE 4975142mN</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="10">
+        <v>2</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="28">
+        <v>43271</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" s="29">
+        <v>43304</v>
+      </c>
+      <c r="L27" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M27" s="10">
+        <v>4</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="P27" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="S27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="T27" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 529723mE 4962865mN</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="10">
+        <v>2</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="28">
+        <v>43271</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" s="29">
+        <v>43304</v>
+      </c>
+      <c r="L28" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M28" s="10">
+        <v>0.20180000000000001</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 529723mE 4962865mN</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="10">
+        <v>7</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="28">
+        <v>43278</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" s="29">
+        <v>43304</v>
+      </c>
+      <c r="L29" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M29" s="10">
+        <v>4</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="O29" s="14" t="s">
+        <v>1014</v>
+      </c>
+      <c r="P29" s="14" t="s">
+        <v>1015</v>
+      </c>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S29" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="T29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 526536mE 4967337mN</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="10">
+        <v>25</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="28">
+        <v>43296</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" s="29">
+        <v>43304</v>
+      </c>
+      <c r="L30" s="30">
+        <v>2018</v>
+      </c>
+      <c r="M30" s="10">
+        <v>2.2016</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>1017</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 525092mE 4967306mN</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="10">
+        <v>1</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="28">
+        <v>43524</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" s="29">
+        <v>43539</v>
+      </c>
+      <c r="L31" s="30">
+        <v>2019</v>
+      </c>
+      <c r="M31" s="10">
+        <v>6</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>1021</v>
+      </c>
+      <c r="O31" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>1023</v>
+      </c>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S31" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="T31" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="0"/>
+        <v>12N 533829mE 4969485mN</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
@@ -4907,13 +7058,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL240"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:N1"/>
+    <sheetView zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -22266,7 +24417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA497"/>
   <sheetViews>
@@ -57692,7 +59843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U61"/>
   <sheetViews>
@@ -60850,7 +63001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE35"/>
   <sheetViews>
@@ -63673,11 +65824,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:P1"/>
     </sheetView>
   </sheetViews>
@@ -70660,7 +72811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AS62"/>
   <sheetViews>
@@ -77491,7 +79642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
@@ -80261,1973 +82412,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:U31"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="36" customFormat="1">
-      <c r="A2" s="31">
-        <v>10</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>909</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="33">
-        <v>42804</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="34">
-        <v>42835</v>
-      </c>
-      <c r="L2" s="35">
-        <v>2017</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>929</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>930</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>931</v>
-      </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>434</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="36" t="str">
-        <f t="shared" ref="U2:U31" si="0">CONCATENATE("12N ",O2,"mE ",P2,"mN")</f>
-        <v>12N 529588mE 4969531mN</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="27" customFormat="1">
-      <c r="A3" s="22">
-        <v>15</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>910</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="24">
-        <v>42807</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K3" s="25">
-        <v>42816</v>
-      </c>
-      <c r="L3" s="26">
-        <v>2017</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>932</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>933</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>934</v>
-      </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23" t="s">
-        <v>434</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 527518mE 4977401mN</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="27" customFormat="1">
-      <c r="A4" s="22">
-        <v>28</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>911</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="24">
-        <v>42819</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K4" s="25">
-        <v>42831</v>
-      </c>
-      <c r="L4" s="26">
-        <v>2017</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>935</v>
-      </c>
-      <c r="O4" s="23" t="s">
-        <v>936</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>937</v>
-      </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23" t="s">
-        <v>434</v>
-      </c>
-      <c r="S4" s="23" t="s">
-        <v>938</v>
-      </c>
-      <c r="T4" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="U4" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 540556mE 4978867mN</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="27" customFormat="1">
-      <c r="A5" s="22">
-        <v>1</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>912</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="24">
-        <v>42866</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K5" s="25">
-        <v>42894</v>
-      </c>
-      <c r="L5" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M5" s="22">
-        <v>3</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>939</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>940</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>941</v>
-      </c>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S5" s="23" t="s">
-        <v>378</v>
-      </c>
-      <c r="T5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 539920mE 4963374mN</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" s="27" customFormat="1">
-      <c r="A6" s="22">
-        <v>6</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>913</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="24">
-        <v>42878</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K6" s="25">
-        <v>42886</v>
-      </c>
-      <c r="L6" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M6" s="22">
-        <v>4</v>
-      </c>
-      <c r="N6" s="23" t="s">
-        <v>942</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>943</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>944</v>
-      </c>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U6" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 543511mE 4963289mN</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="27" customFormat="1">
-      <c r="A7" s="22">
-        <v>8</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>945</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="24">
-        <v>42879</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K7" s="25">
-        <v>42886</v>
-      </c>
-      <c r="L7" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M7" s="22">
-        <v>17</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>946</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>947</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>948</v>
-      </c>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S7" s="23" t="s">
-        <v>378</v>
-      </c>
-      <c r="T7" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U7" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 543062mE 4962326mN</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="27" customFormat="1">
-      <c r="A8" s="22">
-        <v>14</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>914</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="24">
-        <v>42888</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K8" s="25">
-        <v>42942</v>
-      </c>
-      <c r="L8" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M8" s="22">
-        <v>1</v>
-      </c>
-      <c r="N8" s="23" t="s">
-        <v>949</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>950</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>951</v>
-      </c>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="S8" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="T8" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U8" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 530296mE 4961770mN</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="27" customFormat="1">
-      <c r="A9" s="22">
-        <v>15</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>915</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="24">
-        <v>42893</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K9" s="25">
-        <v>42906</v>
-      </c>
-      <c r="L9" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M9" s="22">
-        <v>6</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>952</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>953</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>954</v>
-      </c>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S9" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T9" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U9" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 528094mE 4955737mN</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="27" customFormat="1">
-      <c r="A10" s="22">
-        <v>15</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>916</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="24">
-        <v>42893</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K10" s="25">
-        <v>42906</v>
-      </c>
-      <c r="L10" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M10" s="22">
-        <v>0</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>952</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>953</v>
-      </c>
-      <c r="P10" s="23" t="s">
-        <v>954</v>
-      </c>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S10" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T10" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U10" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 528094mE 4955737mN</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="27" customFormat="1">
-      <c r="A11" s="22">
-        <v>18</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>917</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="24">
-        <v>42897</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K11" s="25">
-        <v>42906</v>
-      </c>
-      <c r="L11" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M11" s="22">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23" t="s">
-        <v>955</v>
-      </c>
-      <c r="O11" s="23" t="s">
-        <v>956</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>957</v>
-      </c>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S11" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="T11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U11" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 526859mE 4955914mN</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="36" customFormat="1">
-      <c r="A12" s="31">
-        <v>20</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>919</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="33">
-        <v>42905</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="K12" s="34">
-        <v>42922</v>
-      </c>
-      <c r="L12" s="35">
-        <v>2017</v>
-      </c>
-      <c r="M12" s="31">
-        <v>8</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>958</v>
-      </c>
-      <c r="O12" s="32" t="s">
-        <v>959</v>
-      </c>
-      <c r="P12" s="32" t="s">
-        <v>960</v>
-      </c>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="S12" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="T12" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="U12" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 527423mE 4962748mN</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="27" customFormat="1">
-      <c r="A13" s="22">
-        <v>22</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>918</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="24">
-        <v>42904</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" s="25">
-        <v>42943</v>
-      </c>
-      <c r="L13" s="26">
-        <v>2017</v>
-      </c>
-      <c r="N13" s="23" t="s">
-        <v>949</v>
-      </c>
-      <c r="O13" s="23" t="s">
-        <v>961</v>
-      </c>
-      <c r="P13" s="23" t="s">
-        <v>962</v>
-      </c>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S13" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T13" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U13" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 529990mE 4965163mN</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="27" customFormat="1">
-      <c r="A14" s="22">
-        <v>23</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>920</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="24">
-        <v>42906</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K14" s="25">
-        <v>42922</v>
-      </c>
-      <c r="L14" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M14" s="22">
-        <v>5</v>
-      </c>
-      <c r="N14" s="23" t="s">
-        <v>963</v>
-      </c>
-      <c r="O14" s="23" t="s">
-        <v>964</v>
-      </c>
-      <c r="P14" s="23" t="s">
-        <v>965</v>
-      </c>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S14" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="T14" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U14" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 526710mE 4963093mN</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="27" customFormat="1">
-      <c r="A15" s="22">
-        <v>23</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>921</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="24">
-        <v>42906</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K15" s="25">
-        <v>42922</v>
-      </c>
-      <c r="L15" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M15" s="22">
-        <v>0</v>
-      </c>
-      <c r="N15" s="23" t="s">
-        <v>963</v>
-      </c>
-      <c r="O15" s="23" t="s">
-        <v>966</v>
-      </c>
-      <c r="P15" s="23" t="s">
-        <v>967</v>
-      </c>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S15" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="T15" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U15" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 526790mE 4963181mN</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="27" customFormat="1">
-      <c r="A16" s="22">
-        <v>30</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>922</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="24">
-        <v>42913</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K16" s="25">
-        <v>42929</v>
-      </c>
-      <c r="L16" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M16" s="22">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>968</v>
-      </c>
-      <c r="O16" s="23" t="s">
-        <v>969</v>
-      </c>
-      <c r="P16" s="23" t="s">
-        <v>970</v>
-      </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="S16" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T16" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U16" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 527049mE 4957506mN</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" s="27" customFormat="1">
-      <c r="A17" s="22">
-        <v>33</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>923</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="24">
-        <v>42918</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K17" s="25">
-        <v>42922</v>
-      </c>
-      <c r="L17" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M17" s="22">
-        <v>0</v>
-      </c>
-      <c r="N17" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="O17" s="23" t="s">
-        <v>972</v>
-      </c>
-      <c r="P17" s="23" t="s">
-        <v>973</v>
-      </c>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="S17" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T17" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U17" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 524166mE 4964425mN</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" s="27" customFormat="1">
-      <c r="A18" s="22">
-        <v>38</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>924</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="24">
-        <v>42922</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="K18" s="25">
-        <v>42929</v>
-      </c>
-      <c r="L18" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M18" s="22">
-        <v>0</v>
-      </c>
-      <c r="N18" s="23" t="s">
-        <v>974</v>
-      </c>
-      <c r="O18" s="23" t="s">
-        <v>975</v>
-      </c>
-      <c r="P18" s="23" t="s">
-        <v>976</v>
-      </c>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="S18" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="T18" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U18" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 526257mE 4955599mN</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" s="27" customFormat="1">
-      <c r="A19" s="22">
-        <v>41</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>925</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="24">
-        <v>42928</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K19" s="25">
-        <v>42941</v>
-      </c>
-      <c r="L19" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M19" s="22">
-        <v>4</v>
-      </c>
-      <c r="N19" s="23" t="s">
-        <v>977</v>
-      </c>
-      <c r="O19" s="23" t="s">
-        <v>978</v>
-      </c>
-      <c r="P19" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="S19" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="T19" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U19" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 533197mE 4958093mN</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" s="27" customFormat="1">
-      <c r="A20" s="22">
-        <v>41</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>926</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>496</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="24">
-        <v>42928</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="K20" s="25">
-        <v>42941</v>
-      </c>
-      <c r="L20" s="26">
-        <v>2017</v>
-      </c>
-      <c r="M20" s="22">
-        <v>0</v>
-      </c>
-      <c r="N20" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="O20" s="23" t="s">
-        <v>981</v>
-      </c>
-      <c r="P20" s="23" t="s">
-        <v>982</v>
-      </c>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="S20" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="T20" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="U20" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 533309mE 4958115mN</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="10">
-        <v>15</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>983</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="28">
-        <v>43071</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="K21" s="29">
-        <v>43079</v>
-      </c>
-      <c r="L21" s="30">
-        <v>2017</v>
-      </c>
-      <c r="M21" s="10">
-        <v>15</v>
-      </c>
-      <c r="N21" s="14" t="s">
-        <v>929</v>
-      </c>
-      <c r="O21" s="14" t="s">
-        <v>984</v>
-      </c>
-      <c r="P21" s="14" t="s">
-        <v>985</v>
-      </c>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="S21" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="T21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="U21" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 529467mE 4970128mN</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="10">
-        <v>1</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>986</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="28">
-        <v>43133</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="29">
-        <v>43160</v>
-      </c>
-      <c r="L22" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M22" s="10">
-        <v>57</v>
-      </c>
-      <c r="N22" s="14" t="s">
-        <v>987</v>
-      </c>
-      <c r="O22" s="14" t="s">
-        <v>988</v>
-      </c>
-      <c r="P22" s="14" t="s">
-        <v>989</v>
-      </c>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U22" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 533055mE 4970931mN</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="A23" s="10">
-        <v>10</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>990</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="28">
-        <v>43156</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" s="29">
-        <v>43168</v>
-      </c>
-      <c r="L23" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M23" s="10">
-        <v>9</v>
-      </c>
-      <c r="N23" s="14" t="s">
-        <v>991</v>
-      </c>
-      <c r="O23" s="14" t="s">
-        <v>992</v>
-      </c>
-      <c r="P23" s="14" t="s">
-        <v>993</v>
-      </c>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14" t="s">
-        <v>994</v>
-      </c>
-      <c r="S23" s="14" t="s">
-        <v>995</v>
-      </c>
-      <c r="T23" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U23" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 546430mE 4969479mN</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="10">
-        <v>18</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>927</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="28">
-        <v>43173</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K24" s="29">
-        <v>43182</v>
-      </c>
-      <c r="L24" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M24" s="10">
-        <v>610</v>
-      </c>
-      <c r="N24" s="14" t="s">
-        <v>996</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>997</v>
-      </c>
-      <c r="P24" s="14" t="s">
-        <v>998</v>
-      </c>
-      <c r="Q24" s="14"/>
-      <c r="T24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U24" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 545270mE 4972924mN</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" s="10">
-        <v>22</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>999</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="28">
-        <v>43177</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K25" s="29">
-        <v>43182</v>
-      </c>
-      <c r="L25" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M25" s="10">
-        <v>0</v>
-      </c>
-      <c r="N25" s="14" t="s">
-        <v>1000</v>
-      </c>
-      <c r="O25" s="14" t="s">
-        <v>1001</v>
-      </c>
-      <c r="P25" s="14" t="s">
-        <v>1002</v>
-      </c>
-      <c r="Q25" s="14"/>
-      <c r="T25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U25" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 542618mE 4975375mN</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="10">
-        <v>22</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H26" s="28">
-        <v>43182</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K26" s="29">
-        <v>43187</v>
-      </c>
-      <c r="L26" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M26" s="10">
-        <v>510</v>
-      </c>
-      <c r="N26" s="14" t="s">
-        <v>1004</v>
-      </c>
-      <c r="O26" s="14" t="s">
-        <v>1005</v>
-      </c>
-      <c r="P26" s="14" t="s">
-        <v>1006</v>
-      </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="T26" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U26" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 542398mE 4975142mN</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="10">
-        <v>2</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="28">
-        <v>43271</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K27" s="29">
-        <v>43304</v>
-      </c>
-      <c r="L27" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M27" s="10">
-        <v>4</v>
-      </c>
-      <c r="N27" s="14" t="s">
-        <v>1008</v>
-      </c>
-      <c r="O27" s="14" t="s">
-        <v>1009</v>
-      </c>
-      <c r="P27" s="14" t="s">
-        <v>1010</v>
-      </c>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="S27" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="T27" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="U27" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 529723mE 4962865mN</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="10">
-        <v>2</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" s="28">
-        <v>43271</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K28" s="29">
-        <v>43304</v>
-      </c>
-      <c r="L28" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M28" s="10">
-        <v>0.20180000000000001</v>
-      </c>
-      <c r="N28" s="14" t="s">
-        <v>1008</v>
-      </c>
-      <c r="O28" s="14" t="s">
-        <v>1009</v>
-      </c>
-      <c r="P28" s="14" t="s">
-        <v>1010</v>
-      </c>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="S28" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="T28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="U28" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 529723mE 4962865mN</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="10">
-        <v>7</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" s="28">
-        <v>43278</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K29" s="29">
-        <v>43304</v>
-      </c>
-      <c r="L29" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M29" s="10">
-        <v>4</v>
-      </c>
-      <c r="N29" s="14" t="s">
-        <v>1013</v>
-      </c>
-      <c r="O29" s="14" t="s">
-        <v>1014</v>
-      </c>
-      <c r="P29" s="14" t="s">
-        <v>1015</v>
-      </c>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="S29" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="T29" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="U29" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 526536mE 4967337mN</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="10">
-        <v>25</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" s="28">
-        <v>43296</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" s="29">
-        <v>43304</v>
-      </c>
-      <c r="L30" s="30">
-        <v>2018</v>
-      </c>
-      <c r="M30" s="10">
-        <v>2.2016</v>
-      </c>
-      <c r="N30" s="14" t="s">
-        <v>1017</v>
-      </c>
-      <c r="O30" s="14" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P30" s="14" t="s">
-        <v>1019</v>
-      </c>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="S30" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="T30" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="U30" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 525092mE 4967306mN</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="10">
-        <v>1</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H31" s="28">
-        <v>43524</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K31" s="29">
-        <v>43539</v>
-      </c>
-      <c r="L31" s="30">
-        <v>2019</v>
-      </c>
-      <c r="M31" s="10">
-        <v>6</v>
-      </c>
-      <c r="N31" s="14" t="s">
-        <v>1021</v>
-      </c>
-      <c r="O31" s="14" t="s">
-        <v>1022</v>
-      </c>
-      <c r="P31" s="14" t="s">
-        <v>1023</v>
-      </c>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="S31" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="T31" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="U31" t="str">
-        <f t="shared" si="0"/>
-        <v>12N 533829mE 4969485mN</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
labeled F207 and F209 kills
</commit_message>
<xml_diff>
--- a/data/Cougars_ODBA_KIlls_Setup.xlsx
+++ b/data/Cougars_ODBA_KIlls_Setup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSU\AI Capstone\ai-capstone\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binde\Git\ai-capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83181875-5609-4A11-B3B7-C3547646D856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0457F6-7D38-42BC-AB86-0EC62A9F3EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="624" windowWidth="22680" windowHeight="11616" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoPlots" sheetId="10" r:id="rId1"/>
@@ -4238,15 +4238,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE45E2E-6649-4C29-87B5-2DB9979F8950}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4368,7 +4368,7 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="19" t="s">
@@ -6334,10 +6334,10 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13:M17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
@@ -6450,8 +6450,12 @@
       <c r="K2" s="4">
         <v>0.93125000000000002</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="L2" s="4">
+        <v>0.9243055555555556</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.92783564814814812</v>
+      </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
@@ -7062,12 +7066,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL240"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
@@ -11758,8 +11762,8 @@
       <c r="L63" s="4">
         <v>0.38101851851851848</v>
       </c>
-      <c r="M63" s="4">
-        <v>0.38137731481481479</v>
+      <c r="M63" s="53">
+        <v>0.38693287037037033</v>
       </c>
       <c r="N63" s="53">
         <v>0.39303240740740741</v>
@@ -14177,7 +14181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:29" ht="31.2">
+    <row r="97" spans="1:29" ht="31">
       <c r="A97" s="8">
         <v>202</v>
       </c>
@@ -14249,7 +14253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:29" ht="31.2">
+    <row r="98" spans="1:29" ht="31">
       <c r="A98" s="8">
         <v>202</v>
       </c>
@@ -14321,7 +14325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="99" spans="1:29" ht="31.2">
+    <row r="99" spans="1:29" ht="31">
       <c r="A99" s="8">
         <v>202</v>
       </c>
@@ -14393,7 +14397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:29" ht="31.2">
+    <row r="100" spans="1:29" ht="31">
       <c r="A100" s="8">
         <v>202</v>
       </c>
@@ -17851,10 +17855,10 @@
         <v>0.24781249999999999</v>
       </c>
       <c r="L147" s="4">
-        <v>0.2507523148148148</v>
+        <v>0.2507638888888889</v>
       </c>
       <c r="M147" s="4">
-        <v>0.25141203703703702</v>
+        <v>0.25128472222222226</v>
       </c>
       <c r="N147" s="4">
         <v>0.2519791666666667</v>
@@ -20094,7 +20098,7 @@
         <v>0.19303240740740743</v>
       </c>
       <c r="M178" s="4">
-        <v>0.19358796296296296</v>
+        <v>0.19359953703703703</v>
       </c>
       <c r="N178" s="53">
         <v>0.20121527777777778</v>
@@ -21852,7 +21856,7 @@
         <v>3.2060185185185185E-2</v>
       </c>
       <c r="N202" s="53">
-        <v>3.3333333333333333E-2</v>
+        <v>3.6400462962962961E-2</v>
       </c>
       <c r="P202" t="s">
         <v>39</v>
@@ -24425,9 +24429,9 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.5"/>
   <cols>
-    <col min="8" max="8" width="11.19921875" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -38472,7 +38476,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="197" spans="1:26" ht="31.2">
+    <row r="197" spans="1:26" ht="31">
       <c r="A197" s="8">
         <v>202</v>
       </c>
@@ -38543,7 +38547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:26" ht="31.2">
+    <row r="198" spans="1:26" ht="31">
       <c r="A198" s="8">
         <v>202</v>
       </c>
@@ -38614,7 +38618,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="199" spans="1:26" ht="31.2">
+    <row r="199" spans="1:26" ht="31">
       <c r="A199" s="8">
         <v>202</v>
       </c>
@@ -38685,7 +38689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="200" spans="1:26" ht="31.2">
+    <row r="200" spans="1:26" ht="31">
       <c r="A200" s="8">
         <v>202</v>
       </c>
@@ -59851,9 +59855,9 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="20" max="20" width="26.19921875" customWidth="1"/>
+    <col min="20" max="20" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -63009,7 +63013,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
@@ -63070,7 +63074,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="37" customFormat="1" ht="15">
+    <row r="2" spans="1:31" s="37" customFormat="1">
       <c r="A2" s="37">
         <v>202</v>
       </c>
@@ -63126,7 +63130,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="37" customFormat="1" ht="15">
+    <row r="3" spans="1:31" s="37" customFormat="1">
       <c r="A3" s="37">
         <v>202</v>
       </c>
@@ -63182,7 +63186,7 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="37" customFormat="1" ht="15">
+    <row r="4" spans="1:31" s="37" customFormat="1">
       <c r="A4" s="37">
         <v>202</v>
       </c>
@@ -65828,11 +65832,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK177"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P1"/>
+    <sheetView topLeftCell="C1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="20" max="20" width="17" customWidth="1"/>
   </cols>
@@ -65957,10 +65961,18 @@
       <c r="L2" s="4">
         <v>0.69722222222222197</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="M2" s="4">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.69738425925925929</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.69755787037037031</v>
+      </c>
+      <c r="P2" s="53">
+        <v>0.70416666666666661</v>
+      </c>
     </row>
     <row r="3" spans="1:37">
       <c r="B3">
@@ -66074,10 +66086,18 @@
       <c r="L5" s="4">
         <v>0.2</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
+      <c r="M5" s="4">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.20011574074074076</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.20017361111111112</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.20098379629629629</v>
+      </c>
     </row>
     <row r="6" spans="1:37">
       <c r="B6">
@@ -66191,10 +66211,18 @@
       <c r="L8" s="4">
         <v>0.21319444444444399</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="M8" s="4">
+        <v>0.20902777777777778</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.21251157407407406</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.21274305555555553</v>
+      </c>
+      <c r="P8" s="53">
+        <v>0.22395833333333334</v>
+      </c>
     </row>
     <row r="9" spans="1:37">
       <c r="B9">
@@ -66308,10 +66336,18 @@
       <c r="L11" s="4">
         <v>0.26736111111111099</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="M11" s="53">
+        <v>0.26319444444444445</v>
+      </c>
+      <c r="N11" s="53">
+        <v>0.26533564814814814</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.26725694444444442</v>
+      </c>
+      <c r="P11" s="53">
+        <v>0.2714699074074074</v>
+      </c>
     </row>
     <row r="12" spans="1:37">
       <c r="B12">
@@ -66425,10 +66461,18 @@
       <c r="L14" s="4">
         <v>0.27986111111111101</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="M14" s="4">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.27976851851851853</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0.28027777777777779</v>
+      </c>
+      <c r="P14" s="53">
+        <v>0.28750000000000003</v>
+      </c>
     </row>
     <row r="15" spans="1:37">
       <c r="B15">
@@ -72819,14 +72863,14 @@
       <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="8" max="8" width="5.796875" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="14" max="14" width="31.296875" customWidth="1"/>
+    <col min="14" max="14" width="31.33203125" customWidth="1"/>
     <col min="17" max="17" width="39.5" customWidth="1"/>
-    <col min="41" max="41" width="18.69921875" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -72960,7 +73004,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="2" spans="1:43" s="27" customFormat="1" ht="403">
       <c r="A2" s="23" t="s">
         <v>361</v>
       </c>
@@ -73191,7 +73235,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;825&lt;br/&gt;313&lt;br/&gt;42810</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="4" spans="1:43" s="27" customFormat="1" ht="403">
       <c r="A4" s="23" t="s">
         <v>361</v>
       </c>
@@ -73320,7 +73364,7 @@
         <v>Elk&lt;br/&gt;Male&lt;br/&gt;Polished&lt;br/&gt;Yearling&lt;br/&gt;Late Winter&lt;br/&gt;824&lt;br/&gt;316&lt;br/&gt;42812</v>
       </c>
     </row>
-    <row r="5" spans="1:43" s="27" customFormat="1" ht="327.60000000000002">
+    <row r="5" spans="1:43" s="27" customFormat="1" ht="294.5">
       <c r="A5" s="23" t="s">
         <v>361</v>
       </c>
@@ -73444,7 +73488,7 @@
 &lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;852&lt;br/&gt;323&lt;br/&gt;42820</v>
       </c>
     </row>
-    <row r="6" spans="1:43" s="27" customFormat="1" ht="249.6">
+    <row r="6" spans="1:43" s="27" customFormat="1" ht="232.5">
       <c r="A6" s="23" t="s">
         <v>361</v>
       </c>
@@ -73675,7 +73719,7 @@
         <v>Grouse&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Unknown&lt;br/&gt;Summer&lt;br/&gt;855&lt;br/&gt;380&lt;br/&gt;42866</v>
       </c>
     </row>
-    <row r="8" spans="1:43" s="27" customFormat="1" ht="202.8">
+    <row r="8" spans="1:43" s="27" customFormat="1" ht="201.5">
       <c r="A8" s="23" t="s">
         <v>361</v>
       </c>
@@ -73795,7 +73839,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Yearling&lt;br/&gt;Summer&lt;br/&gt;856&lt;br/&gt;387&lt;br/&gt;42872</v>
       </c>
     </row>
-    <row r="9" spans="1:43" s="27" customFormat="1" ht="62.4">
+    <row r="9" spans="1:43" s="27" customFormat="1" ht="62">
       <c r="A9" s="23" t="s">
         <v>361</v>
       </c>
@@ -73885,7 +73929,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;864&lt;br/&gt;388&lt;br/&gt;42874</v>
       </c>
     </row>
-    <row r="10" spans="1:43" s="27" customFormat="1" ht="31.2">
+    <row r="10" spans="1:43" s="27" customFormat="1" ht="31">
       <c r="A10" s="23" t="s">
         <v>361</v>
       </c>
@@ -73996,7 +74040,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;828&lt;br/&gt;393&lt;br/&gt;42878</v>
       </c>
     </row>
-    <row r="11" spans="1:43" s="27" customFormat="1" ht="156">
+    <row r="11" spans="1:43" s="27" customFormat="1" ht="155">
       <c r="A11" s="23" t="s">
         <v>361</v>
       </c>
@@ -74104,7 +74148,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;871&lt;br/&gt;395&lt;br/&gt;42880</v>
       </c>
     </row>
-    <row r="12" spans="1:43" s="27" customFormat="1" ht="46.8">
+    <row r="12" spans="1:43" s="27" customFormat="1" ht="46.5">
       <c r="A12" s="23" t="s">
         <v>361</v>
       </c>
@@ -74209,7 +74253,7 @@
         <v>Yellow-Bellied Marmot&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;859&lt;br/&gt;399&lt;br/&gt;42883</v>
       </c>
     </row>
-    <row r="13" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="13" spans="1:43" s="27" customFormat="1" ht="403">
       <c r="A13" s="23" t="s">
         <v>496</v>
       </c>
@@ -74320,7 +74364,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;865&lt;br/&gt;346&lt;br/&gt;42883</v>
       </c>
     </row>
-    <row r="14" spans="1:43" s="27" customFormat="1" ht="62.4">
+    <row r="14" spans="1:43" s="27" customFormat="1" ht="62">
       <c r="A14" s="23" t="s">
         <v>361</v>
       </c>
@@ -74431,7 +74475,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;869&lt;br/&gt;401&lt;br/&gt;42884</v>
       </c>
     </row>
-    <row r="15" spans="1:43" s="27" customFormat="1" ht="46.8">
+    <row r="15" spans="1:43" s="27" customFormat="1" ht="46.5">
       <c r="A15" s="23" t="s">
         <v>361</v>
       </c>
@@ -74542,7 +74586,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;860&lt;br/&gt;402&lt;br/&gt;42885</v>
       </c>
     </row>
-    <row r="16" spans="1:43" s="27" customFormat="1" ht="358.8">
+    <row r="16" spans="1:43" s="27" customFormat="1" ht="325.5">
       <c r="A16" s="23" t="s">
         <v>361</v>
       </c>
@@ -74653,7 +74697,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;862&lt;br/&gt;404&lt;br/&gt;42886</v>
       </c>
     </row>
-    <row r="17" spans="1:43" s="27" customFormat="1" ht="78">
+    <row r="17" spans="1:43" s="27" customFormat="1" ht="77.5">
       <c r="A17" s="23" t="s">
         <v>361</v>
       </c>
@@ -74761,7 +74805,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;861&lt;br/&gt;406&lt;br/&gt;42888</v>
       </c>
     </row>
-    <row r="18" spans="1:43" s="27" customFormat="1" ht="171.6">
+    <row r="18" spans="1:43" s="27" customFormat="1" ht="139.5">
       <c r="A18" s="23" t="s">
         <v>361</v>
       </c>
@@ -74878,7 +74922,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;863&lt;br/&gt;404&lt;br/&gt;42889</v>
       </c>
     </row>
-    <row r="19" spans="1:43" s="27" customFormat="1" ht="265.2">
+    <row r="19" spans="1:43" s="27" customFormat="1" ht="232.5">
       <c r="A19" s="23" t="s">
         <v>361</v>
       </c>
@@ -74980,7 +75024,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;867&lt;br/&gt;409&lt;br/&gt;42891</v>
       </c>
     </row>
-    <row r="20" spans="1:43" s="27" customFormat="1" ht="140.4">
+    <row r="20" spans="1:43" s="27" customFormat="1" ht="124">
       <c r="A20" s="23" t="s">
         <v>361</v>
       </c>
@@ -75088,7 +75132,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;870&lt;br/&gt;411&lt;br/&gt;42892</v>
       </c>
     </row>
-    <row r="21" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="21" spans="1:43" s="27" customFormat="1" ht="387.5">
       <c r="A21" s="23" t="s">
         <v>361</v>
       </c>
@@ -75205,7 +75249,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;868&lt;br/&gt;415&lt;br/&gt;42894</v>
       </c>
     </row>
-    <row r="22" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="22" spans="1:43" s="27" customFormat="1" ht="403">
       <c r="A22" s="23" t="s">
         <v>361</v>
       </c>
@@ -75325,7 +75369,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;874&lt;br/&gt;419&lt;br/&gt;42899</v>
       </c>
     </row>
-    <row r="23" spans="1:43" s="27" customFormat="1" ht="234">
+    <row r="23" spans="1:43" s="27" customFormat="1" ht="232.5">
       <c r="A23" s="23" t="s">
         <v>361</v>
       </c>
@@ -75766,7 +75810,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;831&lt;br/&gt;431&lt;br/&gt;42907</v>
       </c>
     </row>
-    <row r="27" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="27" spans="1:43" s="27" customFormat="1" ht="387.5">
       <c r="A27" s="23" t="s">
         <v>361</v>
       </c>
@@ -75988,7 +76032,7 @@
         <v>Grouse&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Unknown&lt;br/&gt;Summer&lt;br/&gt;883&lt;br/&gt;451&lt;br/&gt;42918</v>
       </c>
     </row>
-    <row r="29" spans="1:43" s="27" customFormat="1" ht="46.8">
+    <row r="29" spans="1:43" s="27" customFormat="1" ht="31">
       <c r="A29" s="23" t="s">
         <v>361</v>
       </c>
@@ -76096,7 +76140,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;884&lt;br/&gt;453&lt;br/&gt;42918</v>
       </c>
     </row>
-    <row r="30" spans="1:43" s="27" customFormat="1" ht="187.2">
+    <row r="30" spans="1:43" s="27" customFormat="1" ht="170.5">
       <c r="A30" s="23" t="s">
         <v>361</v>
       </c>
@@ -76213,7 +76257,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;837&lt;br/&gt;454&lt;br/&gt;42920</v>
       </c>
     </row>
-    <row r="31" spans="1:43" s="27" customFormat="1" ht="280.8">
+    <row r="31" spans="1:43" s="27" customFormat="1" ht="248">
       <c r="A31" s="23" t="s">
         <v>361</v>
       </c>
@@ -76315,7 +76359,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;886&lt;br/&gt;460&lt;br/&gt;42924</v>
       </c>
     </row>
-    <row r="32" spans="1:43" s="27" customFormat="1" ht="374.4">
+    <row r="32" spans="1:43" s="27" customFormat="1" ht="341">
       <c r="A32" s="23" t="s">
         <v>361</v>
       </c>
@@ -76423,7 +76467,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Summer&lt;br/&gt;885&lt;br/&gt;462&lt;br/&gt;42925</v>
       </c>
     </row>
-    <row r="33" spans="1:43" s="27" customFormat="1" ht="46.8">
+    <row r="33" spans="1:43" s="27" customFormat="1" ht="46.5">
       <c r="A33" s="23" t="s">
         <v>361</v>
       </c>
@@ -76534,7 +76578,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;838&lt;br/&gt;466&lt;br/&gt;42929</v>
       </c>
     </row>
-    <row r="34" spans="1:43" s="27" customFormat="1" ht="124.8">
+    <row r="34" spans="1:43" s="27" customFormat="1" ht="124">
       <c r="A34" s="23" t="s">
         <v>361</v>
       </c>
@@ -76642,7 +76686,7 @@
         <v>Pronghorn Antelope&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;892&lt;br/&gt;471&lt;br/&gt;42931</v>
       </c>
     </row>
-    <row r="35" spans="1:43" s="27" customFormat="1" ht="109.2">
+    <row r="35" spans="1:43" s="27" customFormat="1" ht="108.5">
       <c r="A35" s="23" t="s">
         <v>361</v>
       </c>
@@ -76753,7 +76797,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Summer&lt;br/&gt;836&lt;br/&gt;474&lt;br/&gt;42934</v>
       </c>
     </row>
-    <row r="36" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="36" spans="1:43" s="27" customFormat="1" ht="387.5">
       <c r="A36" s="23" t="s">
         <v>361</v>
       </c>
@@ -76876,7 +76920,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Summer&lt;br/&gt;835&lt;br/&gt;476&lt;br/&gt;42935</v>
       </c>
     </row>
-    <row r="37" spans="1:43" s="36" customFormat="1" ht="171.6">
+    <row r="37" spans="1:43" s="36" customFormat="1" ht="155">
       <c r="A37" s="32" t="s">
         <v>361</v>
       </c>
@@ -77113,7 +77157,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Yearling&lt;br/&gt;Early Winter&lt;br/&gt;229&lt;br/&gt;215&lt;br/&gt;43054</v>
       </c>
     </row>
-    <row r="39" spans="1:43" s="27" customFormat="1" ht="327.60000000000002">
+    <row r="39" spans="1:43" s="27" customFormat="1" ht="294.5">
       <c r="A39" s="23" t="s">
         <v>361</v>
       </c>
@@ -77227,7 +77271,7 @@
         <v>Coyote&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Early Winter&lt;br/&gt;228&lt;br/&gt;218&lt;br/&gt;43058</v>
       </c>
     </row>
-    <row r="40" spans="1:43" s="27" customFormat="1" ht="202.8">
+    <row r="40" spans="1:43" s="27" customFormat="1" ht="186">
       <c r="A40" s="23" t="s">
         <v>361</v>
       </c>
@@ -77350,7 +77394,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Adult&lt;br/&gt;Early Winter&lt;br/&gt;230&lt;br/&gt;230&lt;br/&gt;43067</v>
       </c>
     </row>
-    <row r="41" spans="1:43" s="27" customFormat="1" ht="62.4">
+    <row r="41" spans="1:43" s="27" customFormat="1" ht="62">
       <c r="A41" s="23" t="s">
         <v>361</v>
       </c>
@@ -77470,7 +77514,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Calf/fawn&lt;br/&gt;Early Winter&lt;br/&gt;231&lt;br/&gt;233&lt;br/&gt;43070</v>
       </c>
     </row>
-    <row r="42" spans="1:43" s="27" customFormat="1" ht="78">
+    <row r="42" spans="1:43" s="27" customFormat="1" ht="77.5">
       <c r="A42" s="23" t="s">
         <v>361</v>
       </c>
@@ -77701,7 +77745,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Unknown&lt;br/&gt;Early Winter&lt;br/&gt;234&lt;br/&gt;241&lt;br/&gt;43083</v>
       </c>
     </row>
-    <row r="44" spans="1:43" s="27" customFormat="1" ht="327.60000000000002">
+    <row r="44" spans="1:43" s="27" customFormat="1" ht="294.5">
       <c r="A44" s="23" t="s">
         <v>361</v>
       </c>
@@ -77807,7 +77851,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;943&lt;br/&gt;&lt;br/&gt;43151</v>
       </c>
     </row>
-    <row r="45" spans="1:43" s="27" customFormat="1" ht="109.2">
+    <row r="45" spans="1:43" s="27" customFormat="1" ht="108.5">
       <c r="A45" s="23" t="s">
         <v>361</v>
       </c>
@@ -77913,7 +77957,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;953&lt;br/&gt;&lt;br/&gt;43157</v>
       </c>
     </row>
-    <row r="46" spans="1:43" s="27" customFormat="1" ht="358.8">
+    <row r="46" spans="1:43" s="27" customFormat="1" ht="325.5">
       <c r="A46" s="23" t="s">
         <v>361</v>
       </c>
@@ -78010,7 +78054,7 @@
         <v>Red Fox&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Adult&lt;br/&gt;Late Winter&lt;br/&gt;952&lt;br/&gt;&lt;br/&gt;43162</v>
       </c>
     </row>
-    <row r="47" spans="1:43" s="27" customFormat="1" ht="409.6">
+    <row r="47" spans="1:43" s="27" customFormat="1" ht="403">
       <c r="A47" s="23" t="s">
         <v>361</v>
       </c>
@@ -78116,7 +78160,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Late Winter&lt;br/&gt;961&lt;br/&gt;&lt;br/&gt;43163</v>
       </c>
     </row>
-    <row r="48" spans="1:43" s="36" customFormat="1" ht="409.6">
+    <row r="48" spans="1:43" s="36" customFormat="1" ht="403">
       <c r="A48" s="32" t="s">
         <v>361</v>
       </c>
@@ -78228,7 +78272,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Old adult (10+ yrs)&lt;br/&gt;Late Winter&lt;br/&gt;938&lt;br/&gt;&lt;br/&gt;43143</v>
       </c>
     </row>
-    <row r="49" spans="1:45" s="27" customFormat="1" ht="405.6">
+    <row r="49" spans="1:45" s="27" customFormat="1" ht="372">
       <c r="A49" s="23" t="s">
         <v>361</v>
       </c>
@@ -78328,7 +78372,7 @@
         <v>Black-tailed Deer&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;967&lt;br/&gt;&lt;br/&gt;43173</v>
       </c>
     </row>
-    <row r="50" spans="1:45" ht="409.6">
+    <row r="50" spans="1:45" ht="403">
       <c r="A50" s="14" t="s">
         <v>361</v>
       </c>
@@ -78437,7 +78481,7 @@
         <v>Elk&lt;br/&gt;Unknown&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;939&lt;br/&gt;&lt;br/&gt;43177</v>
       </c>
     </row>
-    <row r="51" spans="1:45" s="27" customFormat="1" ht="358.8">
+    <row r="51" spans="1:45" s="27" customFormat="1" ht="325.5">
       <c r="A51" s="23" t="s">
         <v>361</v>
       </c>
@@ -78543,7 +78587,7 @@
         <v>Elk&lt;br/&gt;Female&lt;br/&gt;&lt;br/&gt;Calf/fawn&lt;br/&gt;Late Winter&lt;br/&gt;969&lt;br/&gt;&lt;br/&gt;43178</v>
       </c>
     </row>
-    <row r="52" spans="1:45" ht="409.6">
+    <row r="52" spans="1:45" ht="387.5">
       <c r="A52" s="14" t="s">
         <v>361</v>
       </c>
@@ -78780,7 +78824,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="55" spans="1:45" s="27" customFormat="1" ht="409.6">
+    <row r="55" spans="1:45" s="27" customFormat="1" ht="409.5">
       <c r="A55" s="22">
         <v>18</v>
       </c>
@@ -78887,7 +78931,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="56" spans="1:45" s="27" customFormat="1" ht="156">
+    <row r="56" spans="1:45" s="27" customFormat="1" ht="155">
       <c r="A56" s="22">
         <v>24</v>
       </c>
@@ -78994,7 +79038,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="57" spans="1:45" s="27" customFormat="1" ht="409.6">
+    <row r="57" spans="1:45" s="27" customFormat="1" ht="403">
       <c r="A57" s="22">
         <v>27</v>
       </c>
@@ -79529,7 +79573,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="62" spans="1:45" ht="409.6">
+    <row r="62" spans="1:45" ht="409.5">
       <c r="A62" s="10">
         <v>51</v>
       </c>
@@ -79646,11 +79690,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AJ70"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
@@ -79766,10 +79810,18 @@
       <c r="K2" s="4">
         <v>0.29513888888888901</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="L2" s="4">
+        <v>0.29097222222222224</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.29497685185185185</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.29530092592592594</v>
+      </c>
+      <c r="O2" s="53">
+        <v>0.29583333333333334</v>
+      </c>
     </row>
     <row r="3" spans="1:36">
       <c r="A3">
@@ -79883,10 +79935,18 @@
       <c r="K5" s="4">
         <v>0.23888888888888901</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="L5" s="4">
+        <v>0.23541666666666669</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.23905092592592592</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.23944444444444443</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.23983796296296298</v>
+      </c>
     </row>
     <row r="6" spans="1:36">
       <c r="A6">
@@ -79961,10 +80021,18 @@
       <c r="K7" s="4">
         <v>0.42638888888888898</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="L7" s="4">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.42700231481481482</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.42711805555555554</v>
+      </c>
+      <c r="O7" s="53">
+        <v>0.43107638888888888</v>
+      </c>
     </row>
     <row r="8" spans="1:36">
       <c r="A8">
@@ -80039,10 +80107,18 @@
       <c r="K9" s="4">
         <v>0.40763888888888899</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="L9" s="4">
+        <v>0.40347222222222223</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.40721064814814811</v>
+      </c>
+      <c r="N9" s="53">
+        <v>0.4082175925925926</v>
+      </c>
+      <c r="O9" s="53">
+        <v>0.41035879629629629</v>
+      </c>
     </row>
     <row r="10" spans="1:36">
       <c r="A10">
@@ -80156,10 +80232,18 @@
       <c r="K12" s="4">
         <v>0.36666666666666697</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="L12" s="4">
+        <v>0.36180555555555555</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.36572916666666666</v>
+      </c>
+      <c r="N12" s="53">
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="O12" s="53">
+        <v>0.37118055555555557</v>
+      </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13">

</xml_diff>

<commit_message>
Added support for plotting feed start/stop; initial estimates made for each of the already labeled kills (5 for each female), cells marked as red in the ODBA spreadsheet for review
</commit_message>
<xml_diff>
--- a/data/Cougars_ODBA_KIlls_Setup.xlsx
+++ b/data/Cougars_ODBA_KIlls_Setup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="InfoPlots" sheetId="1" state="visible" r:id="rId2"/>
@@ -4086,7 +4086,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="1" sqref="O202:P202 N19"/>
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4220,7 +4220,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="O202:P202 A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6197,7 +6197,7 @@
   <dimension ref="A1:AL21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="1" sqref="O202:P202 Q1"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6977,10 +6977,10 @@
   </sheetPr>
   <dimension ref="A1:AN240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="O202" activeCellId="0" sqref="O202:P202"/>
+      <selection pane="bottomLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8046875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24844,7 +24844,7 @@
   <dimension ref="A1:AA497"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="1" sqref="O202:P202 K8"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -60278,7 +60278,7 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="O202:P202 C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -63444,7 +63444,7 @@
   <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="O202:P202 K2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66274,8 +66274,8 @@
   </sheetPr>
   <dimension ref="A1:AM177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="O202:P202 Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66372,7 +66372,7 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>352</v>
       </c>
@@ -66421,8 +66421,12 @@
       <c r="P2" s="7" t="n">
         <v>0.704166666666667</v>
       </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
+      <c r="Q2" s="18" t="n">
+        <v>0.704178240740741</v>
+      </c>
+      <c r="R2" s="18" t="n">
+        <v>0.713310185185185</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
@@ -66552,8 +66556,12 @@
       <c r="P5" s="5" t="n">
         <v>0.200983796296296</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
+      <c r="Q5" s="18" t="n">
+        <v>0.204861111111111</v>
+      </c>
+      <c r="R5" s="18" t="n">
+        <v>0.215277777777778</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
@@ -66683,8 +66691,12 @@
       <c r="P8" s="7" t="n">
         <v>0.223958333333333</v>
       </c>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
+      <c r="Q8" s="18" t="n">
+        <v>0.224479166666667</v>
+      </c>
+      <c r="R8" s="18" t="n">
+        <v>0.234027777777778</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
@@ -66768,7 +66780,7 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
     </row>
-    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>209</v>
       </c>
@@ -66814,8 +66826,12 @@
       <c r="P11" s="7" t="n">
         <v>0.271469907407407</v>
       </c>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
+      <c r="Q11" s="18" t="n">
+        <v>0.271527777777778</v>
+      </c>
+      <c r="R11" s="18" t="n">
+        <v>0.278993055555556</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
@@ -66945,8 +66961,12 @@
       <c r="P14" s="7" t="n">
         <v>0.2875</v>
       </c>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
+      <c r="Q14" s="18" t="n">
+        <v>0.288541666666667</v>
+      </c>
+      <c r="R14" s="18" t="n">
+        <v>0.293576388888889</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -73668,7 +73688,7 @@
   <dimension ref="A1:AS62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="1" sqref="O202:P202 Z1"/>
+      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -80506,8 +80526,8 @@
   </sheetPr>
   <dimension ref="A1:AL70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="1" sqref="O202:P202 P9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -80644,8 +80664,12 @@
       <c r="O2" s="7" t="n">
         <v>0.295833333333333</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
+      <c r="P2" s="18" t="n">
+        <v>0.309375</v>
+      </c>
+      <c r="Q2" s="18" t="n">
+        <v>0.315972222222222</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -80775,8 +80799,12 @@
       <c r="O5" s="5" t="n">
         <v>0.239837962962963</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="18" t="n">
+        <v>0.245833333333333</v>
+      </c>
+      <c r="Q5" s="18" t="n">
+        <v>0.25625</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -80819,7 +80847,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>207</v>
       </c>
@@ -80865,8 +80893,12 @@
       <c r="O7" s="7" t="n">
         <v>0.431076388888889</v>
       </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
+      <c r="P7" s="18" t="n">
+        <v>0.431087962962963</v>
+      </c>
+      <c r="Q7" s="18" t="n">
+        <v>0.447916666666667</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -80955,8 +80987,12 @@
       <c r="O9" s="7" t="n">
         <v>0.410358796296296</v>
       </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
+      <c r="P9" s="18" t="n">
+        <v>0.413888888888889</v>
+      </c>
+      <c r="Q9" s="18" t="n">
+        <v>0.428472222222222</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -81086,8 +81122,12 @@
       <c r="O12" s="7" t="n">
         <v>0.371180555555556</v>
       </c>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
+      <c r="P12" s="18" t="n">
+        <v>0.372395833333333</v>
+      </c>
+      <c r="Q12" s="18" t="n">
+        <v>0.381828703703704</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">

</xml_diff>